<commit_message>
update to curren t
</commit_message>
<xml_diff>
--- a/initial_claims/WA/WA_data.xlsx
+++ b/initial_claims/WA/WA_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/Documents/GitHub/coronavirus-unemployment/initial_claims/WA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{310F857A-2A8A-0C44-835A-E591DC6B778D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{15E3D747-1D12-F044-B07B-A6A8F6E962E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="17800" activeTab="1" xr2:uid="{562D1027-AFB3-4396-ADB6-415846CFE289}"/>
+    <workbookView xWindow="-29040" yWindow="0" windowWidth="29040" windowHeight="16000" activeTab="1" xr2:uid="{562D1027-AFB3-4396-ADB6-415846CFE289}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2819" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3170" uniqueCount="104">
   <si>
     <t>CountyFips</t>
   </si>
@@ -331,6 +329,24 @@
   </si>
   <si>
     <t>06/14/20 - 06/20/20</t>
+  </si>
+  <si>
+    <t>Week 25</t>
+  </si>
+  <si>
+    <t>06/21/20 - 06/27/20</t>
+  </si>
+  <si>
+    <t>Week 26</t>
+  </si>
+  <si>
+    <t>06/28/20 - 07/04/20</t>
+  </si>
+  <si>
+    <t>Week 27</t>
+  </si>
+  <si>
+    <t>07/05/20 - 07/11/20</t>
   </si>
 </sst>
 </file>
@@ -805,11 +821,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06ADEB73-ED2F-491E-9C4A-B3C92E8A1A89}">
-  <dimension ref="A1:L937"/>
+  <dimension ref="A1:L1054"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A880" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I927" sqref="I927"/>
+      <pane ySplit="1" topLeftCell="A1021" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I1025" sqref="I1025"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24193,11 +24209,9 @@
         <v>117</v>
       </c>
       <c r="G899">
-        <f>F899-F860</f>
         <v>13</v>
       </c>
       <c r="H899" s="4">
-        <f>F899/F860-1</f>
         <v>0.125</v>
       </c>
     </row>
@@ -24221,11 +24235,9 @@
         <v>23</v>
       </c>
       <c r="G900">
-        <f t="shared" ref="G900:G937" si="0">F900-F861</f>
         <v>8</v>
       </c>
       <c r="H900" s="4">
-        <f t="shared" ref="H900:H937" si="1">F900/F861-1</f>
         <v>0.53333333333333344</v>
       </c>
     </row>
@@ -24249,11 +24261,9 @@
         <v>742</v>
       </c>
       <c r="G901">
-        <f t="shared" si="0"/>
         <v>-48</v>
       </c>
       <c r="H901" s="4">
-        <f t="shared" si="1"/>
         <v>-6.0759493670886067E-2</v>
       </c>
     </row>
@@ -24277,11 +24287,9 @@
         <v>230</v>
       </c>
       <c r="G902">
-        <f t="shared" si="0"/>
         <v>-75</v>
       </c>
       <c r="H902" s="4">
-        <f t="shared" si="1"/>
         <v>-0.24590163934426235</v>
       </c>
     </row>
@@ -24305,11 +24313,9 @@
         <v>195</v>
       </c>
       <c r="G903">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="H903" s="4">
-        <f t="shared" si="1"/>
         <v>0.10795454545454541</v>
       </c>
     </row>
@@ -24333,11 +24339,9 @@
         <v>1336</v>
       </c>
       <c r="G904">
-        <f t="shared" si="0"/>
         <v>121</v>
       </c>
       <c r="H904" s="4">
-        <f t="shared" si="1"/>
         <v>9.9588477366255201E-2</v>
       </c>
     </row>
@@ -24361,11 +24365,9 @@
         <v>7</v>
       </c>
       <c r="G905">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H905" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -24389,11 +24391,9 @@
         <v>330</v>
       </c>
       <c r="G906">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="H906" s="4">
-        <f t="shared" si="1"/>
         <v>6.4516129032258007E-2</v>
       </c>
     </row>
@@ -24417,11 +24417,9 @@
         <v>99</v>
       </c>
       <c r="G907">
-        <f t="shared" si="0"/>
         <v>-59</v>
       </c>
       <c r="H907" s="4">
-        <f t="shared" si="1"/>
         <v>-0.37341772151898733</v>
       </c>
     </row>
@@ -24445,11 +24443,9 @@
         <v>25</v>
       </c>
       <c r="G908">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="H908" s="4">
-        <f t="shared" si="1"/>
         <v>0.78571428571428581</v>
       </c>
     </row>
@@ -24473,11 +24469,9 @@
         <v>473</v>
       </c>
       <c r="G909">
-        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="H909" s="4">
-        <f t="shared" si="1"/>
         <v>0.12085308056872046</v>
       </c>
     </row>
@@ -24501,11 +24495,9 @@
         <v>1</v>
       </c>
       <c r="G910">
-        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="H910" s="4">
-        <f t="shared" si="1"/>
         <v>-0.75</v>
       </c>
     </row>
@@ -24529,11 +24521,9 @@
         <v>392</v>
       </c>
       <c r="G911">
-        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="H911" s="4">
-        <f t="shared" si="1"/>
         <v>7.6923076923076872E-2</v>
       </c>
     </row>
@@ -24557,11 +24547,9 @@
         <v>327</v>
       </c>
       <c r="G912">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H912" s="4">
-        <f t="shared" si="1"/>
         <v>0.14335664335664333</v>
       </c>
     </row>
@@ -24585,11 +24573,9 @@
         <v>208</v>
       </c>
       <c r="G913">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H913" s="4">
-        <f t="shared" si="1"/>
         <v>8.3333333333333259E-2</v>
       </c>
     </row>
@@ -24613,11 +24599,9 @@
         <v>93</v>
       </c>
       <c r="G914">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="H914" s="4">
-        <f t="shared" si="1"/>
         <v>0.40909090909090917</v>
       </c>
     </row>
@@ -24641,11 +24625,9 @@
         <v>8752</v>
       </c>
       <c r="G915">
-        <f t="shared" si="0"/>
         <v>-1</v>
       </c>
       <c r="H915" s="4">
-        <f t="shared" si="1"/>
         <v>-1.1424654404201817E-4</v>
       </c>
     </row>
@@ -24669,11 +24651,9 @@
         <v>744</v>
       </c>
       <c r="G916">
-        <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="H916" s="4">
-        <f t="shared" si="1"/>
         <v>7.9825834542815777E-2</v>
       </c>
     </row>
@@ -24697,11 +24677,9 @@
         <v>181</v>
       </c>
       <c r="G917">
-        <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="H917" s="4">
-        <f t="shared" si="1"/>
         <v>0.29285714285714293</v>
       </c>
     </row>
@@ -24725,11 +24703,9 @@
         <v>52</v>
       </c>
       <c r="G918">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H918" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -24753,11 +24729,9 @@
         <v>290</v>
       </c>
       <c r="G919">
-        <f t="shared" si="0"/>
         <v>44</v>
       </c>
       <c r="H919" s="4">
-        <f t="shared" si="1"/>
         <v>0.17886178861788626</v>
       </c>
     </row>
@@ -24781,11 +24755,9 @@
         <v>20</v>
       </c>
       <c r="G920">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H920" s="4">
-        <f t="shared" si="1"/>
         <v>0.4285714285714286</v>
       </c>
     </row>
@@ -24809,11 +24781,9 @@
         <v>164</v>
       </c>
       <c r="G921">
-        <f t="shared" si="0"/>
         <v>-29</v>
       </c>
       <c r="H921" s="4">
-        <f t="shared" si="1"/>
         <v>-0.15025906735751293</v>
       </c>
     </row>
@@ -24837,11 +24807,9 @@
         <v>109</v>
       </c>
       <c r="G922">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H922" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -24865,11 +24833,9 @@
         <v>58</v>
       </c>
       <c r="G923">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H923" s="4">
-        <f t="shared" si="1"/>
         <v>7.4074074074074181E-2</v>
       </c>
     </row>
@@ -24893,11 +24859,9 @@
         <v>38</v>
       </c>
       <c r="G924">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H924" s="4">
-        <f t="shared" si="1"/>
         <v>8.5714285714285632E-2</v>
       </c>
     </row>
@@ -24921,11 +24885,9 @@
         <v>3702</v>
       </c>
       <c r="G925">
-        <f t="shared" si="0"/>
         <v>120</v>
       </c>
       <c r="H925" s="4">
-        <f t="shared" si="1"/>
         <v>3.350083752093802E-2</v>
       </c>
     </row>
@@ -24949,11 +24911,9 @@
         <v>43</v>
       </c>
       <c r="G926">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H926" s="4">
-        <f t="shared" si="1"/>
         <v>0.16216216216216206</v>
       </c>
     </row>
@@ -24977,11 +24937,9 @@
         <v>502</v>
       </c>
       <c r="G927">
-        <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="H927" s="4">
-        <f t="shared" si="1"/>
         <v>7.2649572649572614E-2</v>
       </c>
     </row>
@@ -25005,11 +24963,9 @@
         <v>37</v>
       </c>
       <c r="G928">
-        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H928" s="4">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -25033,11 +24989,9 @@
         <v>3458</v>
       </c>
       <c r="G929">
-        <f t="shared" si="0"/>
         <v>-239</v>
       </c>
       <c r="H929" s="4">
-        <f t="shared" si="1"/>
         <v>-6.4647011090072981E-2</v>
       </c>
     </row>
@@ -25061,11 +25015,9 @@
         <v>1789</v>
       </c>
       <c r="G930">
-        <f t="shared" si="0"/>
         <v>172</v>
       </c>
       <c r="H930" s="4">
-        <f t="shared" si="1"/>
         <v>0.10636982065553502</v>
       </c>
     </row>
@@ -25089,11 +25041,9 @@
         <v>112</v>
       </c>
       <c r="G931">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="H931" s="4">
-        <f t="shared" si="1"/>
         <v>0.23076923076923084</v>
       </c>
     </row>
@@ -25117,11 +25067,9 @@
         <v>940</v>
       </c>
       <c r="G932">
-        <f t="shared" si="0"/>
         <v>131</v>
       </c>
       <c r="H932" s="4">
-        <f t="shared" si="1"/>
         <v>0.16192830655129797</v>
       </c>
     </row>
@@ -25145,11 +25093,9 @@
         <v>6</v>
       </c>
       <c r="G933">
-        <f t="shared" si="0"/>
         <v>-2</v>
       </c>
       <c r="H933" s="4">
-        <f t="shared" si="1"/>
         <v>-0.25</v>
       </c>
     </row>
@@ -25173,11 +25119,9 @@
         <v>140</v>
       </c>
       <c r="G934">
-        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="H934" s="4">
-        <f t="shared" si="1"/>
         <v>0.30841121495327095</v>
       </c>
     </row>
@@ -25201,11 +25145,9 @@
         <v>952</v>
       </c>
       <c r="G935">
-        <f t="shared" si="0"/>
         <v>-3</v>
       </c>
       <c r="H935" s="4">
-        <f t="shared" si="1"/>
         <v>-3.141361256544517E-3</v>
       </c>
     </row>
@@ -25229,11 +25171,9 @@
         <v>78</v>
       </c>
       <c r="G936">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H936" s="4">
-        <f t="shared" si="1"/>
         <v>5.4054054054053946E-2</v>
       </c>
     </row>
@@ -25257,12 +25197,3052 @@
         <v>1003</v>
       </c>
       <c r="G937">
-        <f t="shared" si="0"/>
         <v>45</v>
       </c>
       <c r="H937" s="4">
-        <f t="shared" si="1"/>
         <v>4.6972860125261029E-2</v>
+      </c>
+    </row>
+    <row r="938" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A938" s="13">
+        <v>1</v>
+      </c>
+      <c r="B938" t="s">
+        <v>7</v>
+      </c>
+      <c r="C938" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D938" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E938" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F938">
+        <v>65</v>
+      </c>
+      <c r="G938">
+        <v>-52</v>
+      </c>
+      <c r="H938" s="4">
+        <v>-0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="939" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A939" s="13">
+        <v>3</v>
+      </c>
+      <c r="B939" t="s">
+        <v>10</v>
+      </c>
+      <c r="C939" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D939" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E939" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F939">
+        <v>29</v>
+      </c>
+      <c r="G939">
+        <v>6</v>
+      </c>
+      <c r="H939" s="4">
+        <v>0.26086956521739135</v>
+      </c>
+    </row>
+    <row r="940" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A940" s="13">
+        <v>5</v>
+      </c>
+      <c r="B940" t="s">
+        <v>11</v>
+      </c>
+      <c r="C940" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D940" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E940" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F940">
+        <v>814</v>
+      </c>
+      <c r="G940">
+        <v>72</v>
+      </c>
+      <c r="H940" s="4">
+        <v>9.7035040431266761E-2</v>
+      </c>
+    </row>
+    <row r="941" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A941" s="13">
+        <v>7</v>
+      </c>
+      <c r="B941" t="s">
+        <v>12</v>
+      </c>
+      <c r="C941" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D941" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E941" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F941">
+        <v>240</v>
+      </c>
+      <c r="G941">
+        <v>10</v>
+      </c>
+      <c r="H941" s="4">
+        <v>4.3478260869565188E-2</v>
+      </c>
+    </row>
+    <row r="942" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A942" s="13">
+        <v>9</v>
+      </c>
+      <c r="B942" t="s">
+        <v>13</v>
+      </c>
+      <c r="C942" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D942" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E942" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F942">
+        <v>258</v>
+      </c>
+      <c r="G942">
+        <v>63</v>
+      </c>
+      <c r="H942" s="4">
+        <v>0.32307692307692304</v>
+      </c>
+    </row>
+    <row r="943" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A943" s="13">
+        <v>11</v>
+      </c>
+      <c r="B943" t="s">
+        <v>14</v>
+      </c>
+      <c r="C943" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D943" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E943" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F943">
+        <v>1357</v>
+      </c>
+      <c r="G943">
+        <v>21</v>
+      </c>
+      <c r="H943" s="4">
+        <v>1.5718562874251552E-2</v>
+      </c>
+    </row>
+    <row r="944" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A944" s="13">
+        <v>13</v>
+      </c>
+      <c r="B944" t="s">
+        <v>15</v>
+      </c>
+      <c r="C944" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D944" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E944" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F944">
+        <v>11</v>
+      </c>
+      <c r="G944">
+        <v>4</v>
+      </c>
+      <c r="H944" s="4">
+        <v>0.5714285714285714</v>
+      </c>
+    </row>
+    <row r="945" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A945" s="13">
+        <v>15</v>
+      </c>
+      <c r="B945" t="s">
+        <v>16</v>
+      </c>
+      <c r="C945" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D945" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E945" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F945">
+        <v>417</v>
+      </c>
+      <c r="G945">
+        <v>87</v>
+      </c>
+      <c r="H945" s="4">
+        <v>0.26363636363636367</v>
+      </c>
+    </row>
+    <row r="946" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A946" s="13">
+        <v>17</v>
+      </c>
+      <c r="B946" t="s">
+        <v>17</v>
+      </c>
+      <c r="C946" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D946" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E946" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F946">
+        <v>116</v>
+      </c>
+      <c r="G946">
+        <v>17</v>
+      </c>
+      <c r="H946" s="4">
+        <v>0.17171717171717171</v>
+      </c>
+    </row>
+    <row r="947" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A947" s="13">
+        <v>19</v>
+      </c>
+      <c r="B947" t="s">
+        <v>18</v>
+      </c>
+      <c r="C947" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D947" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E947" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F947">
+        <v>18</v>
+      </c>
+      <c r="G947">
+        <v>-7</v>
+      </c>
+      <c r="H947" s="4">
+        <v>-0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="948" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A948" s="13">
+        <v>21</v>
+      </c>
+      <c r="B948" t="s">
+        <v>19</v>
+      </c>
+      <c r="C948" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D948" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E948" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F948">
+        <v>453</v>
+      </c>
+      <c r="G948">
+        <v>-20</v>
+      </c>
+      <c r="H948" s="4">
+        <v>-4.228329809725162E-2</v>
+      </c>
+    </row>
+    <row r="949" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A949" s="13">
+        <v>23</v>
+      </c>
+      <c r="B949" t="s">
+        <v>20</v>
+      </c>
+      <c r="C949" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D949" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E949" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F949">
+        <v>4</v>
+      </c>
+      <c r="G949">
+        <v>3</v>
+      </c>
+      <c r="H949" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="950" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A950" s="13">
+        <v>25</v>
+      </c>
+      <c r="B950" t="s">
+        <v>21</v>
+      </c>
+      <c r="C950" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D950" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E950" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F950">
+        <v>354</v>
+      </c>
+      <c r="G950">
+        <v>-38</v>
+      </c>
+      <c r="H950" s="4">
+        <v>-9.6938775510204134E-2</v>
+      </c>
+    </row>
+    <row r="951" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A951" s="13">
+        <v>27</v>
+      </c>
+      <c r="B951" t="s">
+        <v>22</v>
+      </c>
+      <c r="C951" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D951" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E951" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F951">
+        <v>316</v>
+      </c>
+      <c r="G951">
+        <v>-11</v>
+      </c>
+      <c r="H951" s="4">
+        <v>-3.3639143730886834E-2</v>
+      </c>
+    </row>
+    <row r="952" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A952" s="13">
+        <v>29</v>
+      </c>
+      <c r="B952" t="s">
+        <v>23</v>
+      </c>
+      <c r="C952" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D952" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E952" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F952">
+        <v>201</v>
+      </c>
+      <c r="G952">
+        <v>-7</v>
+      </c>
+      <c r="H952" s="4">
+        <v>-3.3653846153846145E-2</v>
+      </c>
+    </row>
+    <row r="953" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A953" s="13">
+        <v>31</v>
+      </c>
+      <c r="B953" t="s">
+        <v>24</v>
+      </c>
+      <c r="C953" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D953" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E953" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F953">
+        <v>101</v>
+      </c>
+      <c r="G953">
+        <v>8</v>
+      </c>
+      <c r="H953" s="4">
+        <v>8.602150537634401E-2</v>
+      </c>
+    </row>
+    <row r="954" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A954" s="13">
+        <v>33</v>
+      </c>
+      <c r="B954" t="s">
+        <v>25</v>
+      </c>
+      <c r="C954" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D954" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E954" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F954">
+        <v>9179</v>
+      </c>
+      <c r="G954">
+        <v>427</v>
+      </c>
+      <c r="H954" s="4">
+        <v>4.8788848263254136E-2</v>
+      </c>
+    </row>
+    <row r="955" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A955" s="13">
+        <v>35</v>
+      </c>
+      <c r="B955" t="s">
+        <v>26</v>
+      </c>
+      <c r="C955" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D955" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E955" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F955">
+        <v>857</v>
+      </c>
+      <c r="G955">
+        <v>113</v>
+      </c>
+      <c r="H955" s="4">
+        <v>0.1518817204301075</v>
+      </c>
+    </row>
+    <row r="956" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A956" s="13">
+        <v>37</v>
+      </c>
+      <c r="B956" t="s">
+        <v>27</v>
+      </c>
+      <c r="C956" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D956" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E956" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F956">
+        <v>189</v>
+      </c>
+      <c r="G956">
+        <v>8</v>
+      </c>
+      <c r="H956" s="4">
+        <v>4.4198895027624419E-2</v>
+      </c>
+    </row>
+    <row r="957" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A957" s="13">
+        <v>39</v>
+      </c>
+      <c r="B957" t="s">
+        <v>28</v>
+      </c>
+      <c r="C957" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D957" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E957" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F957">
+        <v>54</v>
+      </c>
+      <c r="G957">
+        <v>2</v>
+      </c>
+      <c r="H957" s="4">
+        <v>3.8461538461538547E-2</v>
+      </c>
+    </row>
+    <row r="958" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A958" s="13">
+        <v>41</v>
+      </c>
+      <c r="B958" t="s">
+        <v>29</v>
+      </c>
+      <c r="C958" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D958" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E958" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F958">
+        <v>269</v>
+      </c>
+      <c r="G958">
+        <v>-21</v>
+      </c>
+      <c r="H958" s="4">
+        <v>-7.241379310344831E-2</v>
+      </c>
+    </row>
+    <row r="959" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A959" s="13">
+        <v>43</v>
+      </c>
+      <c r="B959" t="s">
+        <v>30</v>
+      </c>
+      <c r="C959" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D959" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E959" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F959">
+        <v>22</v>
+      </c>
+      <c r="G959">
+        <v>2</v>
+      </c>
+      <c r="H959" s="4">
+        <v>0.10000000000000009</v>
+      </c>
+    </row>
+    <row r="960" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A960" s="13">
+        <v>45</v>
+      </c>
+      <c r="B960" t="s">
+        <v>31</v>
+      </c>
+      <c r="C960" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D960" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E960" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F960">
+        <v>185</v>
+      </c>
+      <c r="G960">
+        <v>21</v>
+      </c>
+      <c r="H960" s="4">
+        <v>0.12804878048780477</v>
+      </c>
+    </row>
+    <row r="961" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A961" s="13">
+        <v>47</v>
+      </c>
+      <c r="B961" t="s">
+        <v>32</v>
+      </c>
+      <c r="C961" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D961" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E961" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F961">
+        <v>129</v>
+      </c>
+      <c r="G961">
+        <v>20</v>
+      </c>
+      <c r="H961" s="4">
+        <v>0.1834862385321101</v>
+      </c>
+    </row>
+    <row r="962" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A962" s="13">
+        <v>49</v>
+      </c>
+      <c r="B962" t="s">
+        <v>33</v>
+      </c>
+      <c r="C962" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D962" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E962" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F962">
+        <v>67</v>
+      </c>
+      <c r="G962">
+        <v>9</v>
+      </c>
+      <c r="H962" s="4">
+        <v>0.15517241379310343</v>
+      </c>
+    </row>
+    <row r="963" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A963" s="13">
+        <v>51</v>
+      </c>
+      <c r="B963" t="s">
+        <v>34</v>
+      </c>
+      <c r="C963" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D963" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E963" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F963">
+        <v>62</v>
+      </c>
+      <c r="G963">
+        <v>24</v>
+      </c>
+      <c r="H963" s="4">
+        <v>0.63157894736842102</v>
+      </c>
+    </row>
+    <row r="964" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A964" s="13">
+        <v>53</v>
+      </c>
+      <c r="B964" t="s">
+        <v>35</v>
+      </c>
+      <c r="C964" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D964" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E964" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F964">
+        <v>3950</v>
+      </c>
+      <c r="G964">
+        <v>248</v>
+      </c>
+      <c r="H964" s="4">
+        <v>6.6990815775256563E-2</v>
+      </c>
+    </row>
+    <row r="965" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A965" s="13">
+        <v>55</v>
+      </c>
+      <c r="B965" t="s">
+        <v>36</v>
+      </c>
+      <c r="C965" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D965" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E965" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F965">
+        <v>39</v>
+      </c>
+      <c r="G965">
+        <v>-4</v>
+      </c>
+      <c r="H965" s="4">
+        <v>-9.3023255813953543E-2</v>
+      </c>
+    </row>
+    <row r="966" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A966" s="13">
+        <v>57</v>
+      </c>
+      <c r="B966" t="s">
+        <v>37</v>
+      </c>
+      <c r="C966" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D966" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E966" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F966">
+        <v>573</v>
+      </c>
+      <c r="G966">
+        <v>71</v>
+      </c>
+      <c r="H966" s="4">
+        <v>0.14143426294820727</v>
+      </c>
+    </row>
+    <row r="967" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A967" s="13">
+        <v>59</v>
+      </c>
+      <c r="B967" t="s">
+        <v>38</v>
+      </c>
+      <c r="C967" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D967" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E967" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F967">
+        <v>53</v>
+      </c>
+      <c r="G967">
+        <v>16</v>
+      </c>
+      <c r="H967" s="4">
+        <v>0.43243243243243246</v>
+      </c>
+    </row>
+    <row r="968" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A968" s="13">
+        <v>61</v>
+      </c>
+      <c r="B968" t="s">
+        <v>39</v>
+      </c>
+      <c r="C968" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D968" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E968" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F968">
+        <v>3911</v>
+      </c>
+      <c r="G968">
+        <v>453</v>
+      </c>
+      <c r="H968" s="4">
+        <v>0.13100057836899937</v>
+      </c>
+    </row>
+    <row r="969" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A969" s="13">
+        <v>63</v>
+      </c>
+      <c r="B969" t="s">
+        <v>40</v>
+      </c>
+      <c r="C969" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D969" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E969" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F969">
+        <v>1992</v>
+      </c>
+      <c r="G969">
+        <v>203</v>
+      </c>
+      <c r="H969" s="4">
+        <v>0.11347121296813856</v>
+      </c>
+    </row>
+    <row r="970" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A970" s="13">
+        <v>65</v>
+      </c>
+      <c r="B970" t="s">
+        <v>41</v>
+      </c>
+      <c r="C970" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D970" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E970" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F970">
+        <v>110</v>
+      </c>
+      <c r="G970">
+        <v>-2</v>
+      </c>
+      <c r="H970" s="4">
+        <v>-1.7857142857142905E-2</v>
+      </c>
+    </row>
+    <row r="971" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A971" s="13">
+        <v>67</v>
+      </c>
+      <c r="B971" t="s">
+        <v>42</v>
+      </c>
+      <c r="C971" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D971" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E971" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F971">
+        <v>1033</v>
+      </c>
+      <c r="G971">
+        <v>93</v>
+      </c>
+      <c r="H971" s="4">
+        <v>9.8936170212766017E-2</v>
+      </c>
+    </row>
+    <row r="972" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A972" s="13">
+        <v>69</v>
+      </c>
+      <c r="B972" t="s">
+        <v>43</v>
+      </c>
+      <c r="C972" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D972" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E972" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F972">
+        <v>11</v>
+      </c>
+      <c r="G972">
+        <v>5</v>
+      </c>
+      <c r="H972" s="4">
+        <v>0.83333333333333326</v>
+      </c>
+    </row>
+    <row r="973" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A973" s="13">
+        <v>71</v>
+      </c>
+      <c r="B973" t="s">
+        <v>44</v>
+      </c>
+      <c r="C973" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D973" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E973" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F973">
+        <v>139</v>
+      </c>
+      <c r="G973">
+        <v>-1</v>
+      </c>
+      <c r="H973" s="4">
+        <v>-7.1428571428571175E-3</v>
+      </c>
+    </row>
+    <row r="974" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A974" s="13">
+        <v>73</v>
+      </c>
+      <c r="B974" t="s">
+        <v>45</v>
+      </c>
+      <c r="C974" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D974" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E974" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F974">
+        <v>1091</v>
+      </c>
+      <c r="G974">
+        <v>139</v>
+      </c>
+      <c r="H974" s="4">
+        <v>0.14600840336134446</v>
+      </c>
+    </row>
+    <row r="975" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A975" s="13">
+        <v>75</v>
+      </c>
+      <c r="B975" t="s">
+        <v>46</v>
+      </c>
+      <c r="C975" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D975" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E975" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F975">
+        <v>85</v>
+      </c>
+      <c r="G975">
+        <v>7</v>
+      </c>
+      <c r="H975" s="4">
+        <v>8.9743589743589647E-2</v>
+      </c>
+    </row>
+    <row r="976" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A976" s="13">
+        <v>77</v>
+      </c>
+      <c r="B976" t="s">
+        <v>47</v>
+      </c>
+      <c r="C976" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D976" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E976" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F976">
+        <v>1077</v>
+      </c>
+      <c r="G976">
+        <v>74</v>
+      </c>
+      <c r="H976" s="4">
+        <v>7.3778664007976058E-2</v>
+      </c>
+    </row>
+    <row r="977" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A977" s="13">
+        <v>1</v>
+      </c>
+      <c r="B977" t="s">
+        <v>7</v>
+      </c>
+      <c r="C977" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D977" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E977" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F977">
+        <v>109</v>
+      </c>
+      <c r="G977">
+        <v>44</v>
+      </c>
+      <c r="H977" s="4">
+        <v>0.67692307692307696</v>
+      </c>
+    </row>
+    <row r="978" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A978" s="13">
+        <v>3</v>
+      </c>
+      <c r="B978" t="s">
+        <v>10</v>
+      </c>
+      <c r="C978" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D978" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E978" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F978">
+        <v>23</v>
+      </c>
+      <c r="G978">
+        <v>-6</v>
+      </c>
+      <c r="H978" s="4">
+        <v>-0.2068965517241379</v>
+      </c>
+    </row>
+    <row r="979" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A979" s="13">
+        <v>5</v>
+      </c>
+      <c r="B979" t="s">
+        <v>11</v>
+      </c>
+      <c r="C979" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D979" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E979" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F979">
+        <v>683</v>
+      </c>
+      <c r="G979">
+        <v>-131</v>
+      </c>
+      <c r="H979" s="4">
+        <v>-0.1609336609336609</v>
+      </c>
+    </row>
+    <row r="980" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A980" s="13">
+        <v>7</v>
+      </c>
+      <c r="B980" t="s">
+        <v>12</v>
+      </c>
+      <c r="C980" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D980" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E980" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F980">
+        <v>239</v>
+      </c>
+      <c r="G980">
+        <v>-1</v>
+      </c>
+      <c r="H980" s="4">
+        <v>-4.1666666666666519E-3</v>
+      </c>
+    </row>
+    <row r="981" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A981" s="13">
+        <v>9</v>
+      </c>
+      <c r="B981" t="s">
+        <v>13</v>
+      </c>
+      <c r="C981" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D981" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E981" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F981">
+        <v>207</v>
+      </c>
+      <c r="G981">
+        <v>-51</v>
+      </c>
+      <c r="H981" s="4">
+        <v>-0.19767441860465118</v>
+      </c>
+    </row>
+    <row r="982" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A982" s="13">
+        <v>11</v>
+      </c>
+      <c r="B982" t="s">
+        <v>14</v>
+      </c>
+      <c r="C982" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D982" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E982" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F982">
+        <v>1411</v>
+      </c>
+      <c r="G982">
+        <v>54</v>
+      </c>
+      <c r="H982" s="4">
+        <v>3.9793662490788417E-2</v>
+      </c>
+    </row>
+    <row r="983" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A983" s="13">
+        <v>13</v>
+      </c>
+      <c r="B983" t="s">
+        <v>15</v>
+      </c>
+      <c r="C983" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D983" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E983" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F983">
+        <v>11</v>
+      </c>
+      <c r="G983">
+        <v>0</v>
+      </c>
+      <c r="H983" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="984" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A984" s="13">
+        <v>15</v>
+      </c>
+      <c r="B984" t="s">
+        <v>16</v>
+      </c>
+      <c r="C984" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D984" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E984" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F984">
+        <v>365</v>
+      </c>
+      <c r="G984">
+        <v>-52</v>
+      </c>
+      <c r="H984" s="4">
+        <v>-0.12470023980815348</v>
+      </c>
+    </row>
+    <row r="985" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A985" s="13">
+        <v>17</v>
+      </c>
+      <c r="B985" t="s">
+        <v>17</v>
+      </c>
+      <c r="C985" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D985" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E985" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F985">
+        <v>106</v>
+      </c>
+      <c r="G985">
+        <v>-10</v>
+      </c>
+      <c r="H985" s="4">
+        <v>-8.6206896551724088E-2</v>
+      </c>
+    </row>
+    <row r="986" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A986" s="13">
+        <v>19</v>
+      </c>
+      <c r="B986" t="s">
+        <v>18</v>
+      </c>
+      <c r="C986" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D986" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E986" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F986">
+        <v>19</v>
+      </c>
+      <c r="G986">
+        <v>1</v>
+      </c>
+      <c r="H986" s="4">
+        <v>5.555555555555558E-2</v>
+      </c>
+    </row>
+    <row r="987" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A987" s="13">
+        <v>21</v>
+      </c>
+      <c r="B987" t="s">
+        <v>19</v>
+      </c>
+      <c r="C987" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D987" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E987" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F987">
+        <v>369</v>
+      </c>
+      <c r="G987">
+        <v>-84</v>
+      </c>
+      <c r="H987" s="4">
+        <v>-0.18543046357615889</v>
+      </c>
+    </row>
+    <row r="988" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A988" s="13">
+        <v>23</v>
+      </c>
+      <c r="B988" t="s">
+        <v>20</v>
+      </c>
+      <c r="C988" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D988" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E988" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F988">
+        <v>4</v>
+      </c>
+      <c r="G988">
+        <v>0</v>
+      </c>
+      <c r="H988" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="989" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A989" s="13">
+        <v>25</v>
+      </c>
+      <c r="B989" t="s">
+        <v>21</v>
+      </c>
+      <c r="C989" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D989" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E989" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F989">
+        <v>277</v>
+      </c>
+      <c r="G989">
+        <v>-77</v>
+      </c>
+      <c r="H989" s="4">
+        <v>-0.21751412429378536</v>
+      </c>
+    </row>
+    <row r="990" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A990" s="13">
+        <v>27</v>
+      </c>
+      <c r="B990" t="s">
+        <v>22</v>
+      </c>
+      <c r="C990" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D990" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E990" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F990">
+        <v>255</v>
+      </c>
+      <c r="G990">
+        <v>-61</v>
+      </c>
+      <c r="H990" s="4">
+        <v>-0.19303797468354433</v>
+      </c>
+    </row>
+    <row r="991" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A991" s="13">
+        <v>29</v>
+      </c>
+      <c r="B991" t="s">
+        <v>23</v>
+      </c>
+      <c r="C991" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D991" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E991" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F991">
+        <v>188</v>
+      </c>
+      <c r="G991">
+        <v>-13</v>
+      </c>
+      <c r="H991" s="4">
+        <v>-6.4676616915422924E-2</v>
+      </c>
+    </row>
+    <row r="992" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A992" s="13">
+        <v>31</v>
+      </c>
+      <c r="B992" t="s">
+        <v>24</v>
+      </c>
+      <c r="C992" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D992" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E992" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F992">
+        <v>88</v>
+      </c>
+      <c r="G992">
+        <v>-13</v>
+      </c>
+      <c r="H992" s="4">
+        <v>-0.12871287128712872</v>
+      </c>
+    </row>
+    <row r="993" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A993" s="13">
+        <v>33</v>
+      </c>
+      <c r="B993" t="s">
+        <v>25</v>
+      </c>
+      <c r="C993" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D993" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E993" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F993">
+        <v>7945</v>
+      </c>
+      <c r="G993">
+        <v>-1234</v>
+      </c>
+      <c r="H993" s="4">
+        <v>-0.13443730253840291</v>
+      </c>
+    </row>
+    <row r="994" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A994" s="13">
+        <v>35</v>
+      </c>
+      <c r="B994" t="s">
+        <v>26</v>
+      </c>
+      <c r="C994" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D994" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E994" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F994">
+        <v>697</v>
+      </c>
+      <c r="G994">
+        <v>-160</v>
+      </c>
+      <c r="H994" s="4">
+        <v>-0.18669778296382733</v>
+      </c>
+    </row>
+    <row r="995" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A995" s="13">
+        <v>37</v>
+      </c>
+      <c r="B995" t="s">
+        <v>27</v>
+      </c>
+      <c r="C995" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D995" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E995" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F995">
+        <v>180</v>
+      </c>
+      <c r="G995">
+        <v>-9</v>
+      </c>
+      <c r="H995" s="4">
+        <v>-4.7619047619047672E-2</v>
+      </c>
+    </row>
+    <row r="996" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A996" s="13">
+        <v>39</v>
+      </c>
+      <c r="B996" t="s">
+        <v>28</v>
+      </c>
+      <c r="C996" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D996" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E996" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F996">
+        <v>47</v>
+      </c>
+      <c r="G996">
+        <v>-7</v>
+      </c>
+      <c r="H996" s="4">
+        <v>-0.12962962962962965</v>
+      </c>
+    </row>
+    <row r="997" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A997" s="13">
+        <v>41</v>
+      </c>
+      <c r="B997" t="s">
+        <v>29</v>
+      </c>
+      <c r="C997" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D997" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E997" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F997">
+        <v>247</v>
+      </c>
+      <c r="G997">
+        <v>-22</v>
+      </c>
+      <c r="H997" s="4">
+        <v>-8.1784386617100413E-2</v>
+      </c>
+    </row>
+    <row r="998" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A998" s="13">
+        <v>43</v>
+      </c>
+      <c r="B998" t="s">
+        <v>30</v>
+      </c>
+      <c r="C998" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D998" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E998" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F998">
+        <v>25</v>
+      </c>
+      <c r="G998">
+        <v>3</v>
+      </c>
+      <c r="H998" s="4">
+        <v>0.13636363636363646</v>
+      </c>
+    </row>
+    <row r="999" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A999" s="13">
+        <v>45</v>
+      </c>
+      <c r="B999" t="s">
+        <v>31</v>
+      </c>
+      <c r="C999" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D999" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E999" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F999">
+        <v>188</v>
+      </c>
+      <c r="G999">
+        <v>3</v>
+      </c>
+      <c r="H999" s="4">
+        <v>1.6216216216216273E-2</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1000" s="13">
+        <v>47</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1000" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1000" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1000" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1000">
+        <v>115</v>
+      </c>
+      <c r="G1000">
+        <v>-14</v>
+      </c>
+      <c r="H1000" s="4">
+        <v>-0.10852713178294571</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1001" s="13">
+        <v>49</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1001" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1001" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1001" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1001">
+        <v>50</v>
+      </c>
+      <c r="G1001">
+        <v>-17</v>
+      </c>
+      <c r="H1001" s="4">
+        <v>-0.25373134328358204</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1002" s="13">
+        <v>51</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1002" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1002" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1002" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1002">
+        <v>54</v>
+      </c>
+      <c r="G1002">
+        <v>-8</v>
+      </c>
+      <c r="H1002" s="4">
+        <v>-0.12903225806451613</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1003" s="13">
+        <v>53</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1003" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1003" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1003" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1003">
+        <v>3509</v>
+      </c>
+      <c r="G1003">
+        <v>-441</v>
+      </c>
+      <c r="H1003" s="4">
+        <v>-0.11164556962025318</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1004" s="13">
+        <v>55</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1004" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1004" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1004" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1004">
+        <v>43</v>
+      </c>
+      <c r="G1004">
+        <v>4</v>
+      </c>
+      <c r="H1004" s="4">
+        <v>0.10256410256410264</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1005" s="13">
+        <v>57</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1005" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1005" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1005" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1005">
+        <v>449</v>
+      </c>
+      <c r="G1005">
+        <v>-124</v>
+      </c>
+      <c r="H1005" s="4">
+        <v>-0.21640488656195467</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1006" s="13">
+        <v>59</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1006" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1006" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1006" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1006">
+        <v>42</v>
+      </c>
+      <c r="G1006">
+        <v>-11</v>
+      </c>
+      <c r="H1006" s="4">
+        <v>-0.20754716981132071</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1007" s="13">
+        <v>61</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1007" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1007" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1007" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1007">
+        <v>3262</v>
+      </c>
+      <c r="G1007">
+        <v>-649</v>
+      </c>
+      <c r="H1007" s="4">
+        <v>-0.16594221426745082</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1008" s="13">
+        <v>63</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1008" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1008" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1008" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1008">
+        <v>1989</v>
+      </c>
+      <c r="G1008">
+        <v>-3</v>
+      </c>
+      <c r="H1008" s="4">
+        <v>-1.5060240963855609E-3</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1009" s="13">
+        <v>65</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1009" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1009" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1009" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1009">
+        <v>108</v>
+      </c>
+      <c r="G1009">
+        <v>-2</v>
+      </c>
+      <c r="H1009" s="4">
+        <v>-1.8181818181818188E-2</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1010" s="13">
+        <v>67</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1010" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1010" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1010" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1010">
+        <v>1121</v>
+      </c>
+      <c r="G1010">
+        <v>88</v>
+      </c>
+      <c r="H1010" s="4">
+        <v>8.5188770571152039E-2</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1011" s="13">
+        <v>69</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1011" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1011" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1011" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1011">
+        <v>7</v>
+      </c>
+      <c r="G1011">
+        <v>-4</v>
+      </c>
+      <c r="H1011" s="4">
+        <v>-0.36363636363636365</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1012" s="13">
+        <v>71</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1012" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1012" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1012" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1012">
+        <v>115</v>
+      </c>
+      <c r="G1012">
+        <v>-24</v>
+      </c>
+      <c r="H1012" s="4">
+        <v>-0.17266187050359716</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1013" s="13">
+        <v>73</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1013" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1013" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1013" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1013">
+        <v>982</v>
+      </c>
+      <c r="G1013">
+        <v>-109</v>
+      </c>
+      <c r="H1013" s="4">
+        <v>-9.9908340971585741E-2</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1014" s="13">
+        <v>75</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1014" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1014" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1014" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1014">
+        <v>36</v>
+      </c>
+      <c r="G1014">
+        <v>-49</v>
+      </c>
+      <c r="H1014" s="4">
+        <v>-0.57647058823529407</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1015" s="13">
+        <v>77</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1015" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1015" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1015" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1015">
+        <v>982</v>
+      </c>
+      <c r="G1015">
+        <v>-95</v>
+      </c>
+      <c r="H1015" s="4">
+        <v>-8.8207985143918255E-2</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1016" s="13">
+        <v>1</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1016" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1016" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1016" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1016">
+        <v>109</v>
+      </c>
+      <c r="G1016">
+        <v>0</v>
+      </c>
+      <c r="H1016" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1017" s="13">
+        <v>3</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1017" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1017" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1017" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1017">
+        <v>33</v>
+      </c>
+      <c r="G1017">
+        <v>10</v>
+      </c>
+      <c r="H1017" s="4">
+        <v>0.43478260869565211</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1018" s="13">
+        <v>5</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1018" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1018" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1018" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1018">
+        <v>934</v>
+      </c>
+      <c r="G1018">
+        <v>251</v>
+      </c>
+      <c r="H1018" s="4">
+        <v>0.36749633967789164</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1019" s="13">
+        <v>7</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1019" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1019" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1019" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1019">
+        <v>366</v>
+      </c>
+      <c r="G1019">
+        <v>127</v>
+      </c>
+      <c r="H1019" s="4">
+        <v>0.53138075313807542</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1020" s="13">
+        <v>9</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1020" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1020" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1020" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1020">
+        <v>317</v>
+      </c>
+      <c r="G1020">
+        <v>110</v>
+      </c>
+      <c r="H1020" s="4">
+        <v>0.5314009661835748</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1021" s="13">
+        <v>11</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1021" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1021" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1021" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1021">
+        <v>1911</v>
+      </c>
+      <c r="G1021">
+        <v>500</v>
+      </c>
+      <c r="H1021" s="4">
+        <v>0.35435861091424514</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1022" s="13">
+        <v>13</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1022" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1022" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1022" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1022">
+        <v>13</v>
+      </c>
+      <c r="G1022">
+        <v>2</v>
+      </c>
+      <c r="H1022" s="4">
+        <v>0.18181818181818188</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1023" s="13">
+        <v>15</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1023" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1023" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1023" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1023">
+        <v>526</v>
+      </c>
+      <c r="G1023">
+        <v>161</v>
+      </c>
+      <c r="H1023" s="4">
+        <v>0.44109589041095898</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1024" s="13">
+        <v>17</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1024" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1024" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1024" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1024">
+        <v>178</v>
+      </c>
+      <c r="G1024">
+        <v>72</v>
+      </c>
+      <c r="H1024" s="4">
+        <v>0.679245283018868</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1025" s="13">
+        <v>19</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1025" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1025" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1025" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1025">
+        <v>13</v>
+      </c>
+      <c r="G1025">
+        <v>-6</v>
+      </c>
+      <c r="H1025" s="4">
+        <v>-0.31578947368421051</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1026" s="13">
+        <v>21</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1026" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1026" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1026" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1026">
+        <v>448</v>
+      </c>
+      <c r="G1026">
+        <v>79</v>
+      </c>
+      <c r="H1026" s="4">
+        <v>0.21409214092140916</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1027" s="13">
+        <v>23</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1027" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1027" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1027" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1027">
+        <v>8</v>
+      </c>
+      <c r="G1027">
+        <v>4</v>
+      </c>
+      <c r="H1027" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1028" s="13">
+        <v>25</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1028" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1028" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1028" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1028">
+        <v>485</v>
+      </c>
+      <c r="G1028">
+        <v>208</v>
+      </c>
+      <c r="H1028" s="4">
+        <v>0.75090252707581229</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1029" s="13">
+        <v>27</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1029" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1029" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1029" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1029">
+        <v>443</v>
+      </c>
+      <c r="G1029">
+        <v>188</v>
+      </c>
+      <c r="H1029" s="4">
+        <v>0.73725490196078436</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1030" s="13">
+        <v>29</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1030" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1030" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1030" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1030">
+        <v>304</v>
+      </c>
+      <c r="G1030">
+        <v>116</v>
+      </c>
+      <c r="H1030" s="4">
+        <v>0.61702127659574457</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1031" s="13">
+        <v>31</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1031" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1031" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1031" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1031">
+        <v>159</v>
+      </c>
+      <c r="G1031">
+        <v>71</v>
+      </c>
+      <c r="H1031" s="4">
+        <v>0.80681818181818188</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1032" s="13">
+        <v>33</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1032" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1032" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1032" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1032">
+        <v>11375</v>
+      </c>
+      <c r="G1032">
+        <v>3430</v>
+      </c>
+      <c r="H1032" s="4">
+        <v>0.43171806167400884</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1033" s="13">
+        <v>35</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1033" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1033" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1033" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1033">
+        <v>1139</v>
+      </c>
+      <c r="G1033">
+        <v>442</v>
+      </c>
+      <c r="H1033" s="4">
+        <v>0.63414634146341453</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1034" s="13">
+        <v>37</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1034" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1034" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1034" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1034">
+        <v>499</v>
+      </c>
+      <c r="G1034">
+        <v>319</v>
+      </c>
+      <c r="H1034" s="4">
+        <v>1.7722222222222221</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1035" s="13">
+        <v>39</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1035" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1035" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1035" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1035">
+        <v>72</v>
+      </c>
+      <c r="G1035">
+        <v>25</v>
+      </c>
+      <c r="H1035" s="4">
+        <v>0.53191489361702127</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1036" s="13">
+        <v>41</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1036" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1036" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1036" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1036">
+        <v>398</v>
+      </c>
+      <c r="G1036">
+        <v>151</v>
+      </c>
+      <c r="H1036" s="4">
+        <v>0.61133603238866407</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1037" s="13">
+        <v>43</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1037" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1037" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1037" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1037">
+        <v>25</v>
+      </c>
+      <c r="G1037">
+        <v>0</v>
+      </c>
+      <c r="H1037" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1038" s="13">
+        <v>45</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1038" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1038" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1038" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1038">
+        <v>317</v>
+      </c>
+      <c r="G1038">
+        <v>129</v>
+      </c>
+      <c r="H1038" s="4">
+        <v>0.68617021276595747</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1039" s="13">
+        <v>47</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1039" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1039" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1039" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1039">
+        <v>155</v>
+      </c>
+      <c r="G1039">
+        <v>40</v>
+      </c>
+      <c r="H1039" s="4">
+        <v>0.34782608695652173</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1040" s="13">
+        <v>49</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1040" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1040" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1040" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1040">
+        <v>93</v>
+      </c>
+      <c r="G1040">
+        <v>43</v>
+      </c>
+      <c r="H1040" s="4">
+        <v>0.8600000000000001</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1041" s="13">
+        <v>51</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1041" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1041" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1041" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1041">
+        <v>66</v>
+      </c>
+      <c r="G1041">
+        <v>12</v>
+      </c>
+      <c r="H1041" s="4">
+        <v>0.22222222222222232</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1042" s="13">
+        <v>53</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1042" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1042" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1042" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1042">
+        <v>5022</v>
+      </c>
+      <c r="G1042">
+        <v>1513</v>
+      </c>
+      <c r="H1042" s="4">
+        <v>0.43117697349672279</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1043" s="13">
+        <v>55</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1043" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1043" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1043" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1043">
+        <v>75</v>
+      </c>
+      <c r="G1043">
+        <v>32</v>
+      </c>
+      <c r="H1043" s="4">
+        <v>0.7441860465116279</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1044" s="13">
+        <v>57</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1044" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1044" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1044" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1044">
+        <v>616</v>
+      </c>
+      <c r="G1044">
+        <v>167</v>
+      </c>
+      <c r="H1044" s="4">
+        <v>0.37193763919821832</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1045" s="13">
+        <v>59</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1045" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1045" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1045" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1045">
+        <v>54</v>
+      </c>
+      <c r="G1045">
+        <v>12</v>
+      </c>
+      <c r="H1045" s="4">
+        <v>0.28571428571428581</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1046" s="13">
+        <v>61</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1046" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1046" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1046" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1046">
+        <v>4614</v>
+      </c>
+      <c r="G1046">
+        <v>1352</v>
+      </c>
+      <c r="H1046" s="4">
+        <v>0.4144696505211527</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1047" s="13">
+        <v>63</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1047" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1047" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1047" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1047">
+        <v>2617</v>
+      </c>
+      <c r="G1047">
+        <v>628</v>
+      </c>
+      <c r="H1047" s="4">
+        <v>0.31573655103066867</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1048" s="13">
+        <v>65</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1048" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1048" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1048" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1048">
+        <v>148</v>
+      </c>
+      <c r="G1048">
+        <v>40</v>
+      </c>
+      <c r="H1048" s="4">
+        <v>0.37037037037037046</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1049" s="13">
+        <v>67</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1049" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1049" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1049" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1049">
+        <v>1521</v>
+      </c>
+      <c r="G1049">
+        <v>400</v>
+      </c>
+      <c r="H1049" s="4">
+        <v>0.35682426404995549</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1050" s="13">
+        <v>69</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1050" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1050" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1050" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1050">
+        <v>10</v>
+      </c>
+      <c r="G1050">
+        <v>3</v>
+      </c>
+      <c r="H1050" s="4">
+        <v>0.4285714285714286</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1051" s="13">
+        <v>71</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1051" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1051" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1051" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1051">
+        <v>202</v>
+      </c>
+      <c r="G1051">
+        <v>87</v>
+      </c>
+      <c r="H1051" s="4">
+        <v>0.75652173913043486</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1052" s="13">
+        <v>73</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1052" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1052" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1052" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1052">
+        <v>1361</v>
+      </c>
+      <c r="G1052">
+        <v>379</v>
+      </c>
+      <c r="H1052" s="4">
+        <v>0.38594704684317716</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1053" s="13">
+        <v>75</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1053" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1053" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1053" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1053">
+        <v>110</v>
+      </c>
+      <c r="G1053">
+        <v>74</v>
+      </c>
+      <c r="H1053" s="4">
+        <v>2.0555555555555554</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1054" s="13">
+        <v>77</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1054" s="3">
+        <v>2020</v>
+      </c>
+      <c r="D1054" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1054" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1054">
+        <v>1314</v>
+      </c>
+      <c r="G1054">
+        <v>332</v>
+      </c>
+      <c r="H1054" s="4">
+        <v>0.33808553971486766</v>
       </c>
     </row>
   </sheetData>

</xml_diff>